<commit_message>
Included whether molecular profiling was before or after radiation treatment
</commit_message>
<xml_diff>
--- a/Lewis et al. Datasets/Dataset 1.xlsx
+++ b/Lewis et al. Datasets/Dataset 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Desktop\FBA-pipeline\Lewis et al. Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA41E5C8-1EF0-476C-BA8E-B76906BC3E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBF44B9-4368-4F62-B5E1-1F7C8F9626A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4298,9 +4298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U918"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>

</xml_diff>